<commit_message>
Tentative de lecture des fichiers
</commit_message>
<xml_diff>
--- a/Interessant/Infos.xlsx
+++ b/Interessant/Infos.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="58">
   <si>
     <t>Instruction</t>
   </si>
@@ -193,6 +192,12 @@
   </si>
   <si>
     <t>ROTR</t>
+  </si>
+  <si>
+    <t>Func (dec)</t>
+  </si>
+  <si>
+    <t>Opcode(dec)</t>
   </si>
 </sst>
 </file>
@@ -227,7 +232,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -354,11 +359,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -382,9 +400,6 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -392,14 +407,49 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -413,18 +463,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="__Anonymous_Sheet_DB__0" displayName="__Anonymous_Sheet_DB__0" ref="A1:E27" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="__Anonymous_Sheet_DB__0" displayName="__Anonymous_Sheet_DB__0" ref="A1:F27" totalsRowShown="0">
   <sortState ref="A2:E26">
     <sortCondition ref="B2:B27"/>
     <sortCondition ref="C2:C27"/>
     <sortCondition ref="D2:D27"/>
   </sortState>
-  <tableColumns count="5">
+  <tableColumns count="6">
     <tableColumn id="1" name="Instruction"/>
     <tableColumn id="2" name="Format"/>
     <tableColumn id="3" name="Opcode (hex)"/>
     <tableColumn id="4" name="Opcode (bin)">
       <calculatedColumnFormula>HEX2BIN(C2,6)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="Opcode(dec)" dataDxfId="0">
+      <calculatedColumnFormula>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Opcode (hex)]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="Func (hex)"/>
   </tableColumns>
@@ -695,15 +748,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -716,14 +769,20 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -737,10 +796,15 @@
         <f t="shared" ref="D2:D27" si="0">HEX2BIN(C2,6)</f>
         <v>000110</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" s="13">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Opcode (hex)]])</f>
+        <v>6</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -754,10 +818,15 @@
         <f t="shared" si="0"/>
         <v>000111</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E3" s="13">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Opcode (hex)]])</f>
+        <v>7</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -771,10 +840,15 @@
         <f t="shared" si="0"/>
         <v>100011</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="8"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4" s="13">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Opcode (hex)]])</f>
+        <v>35</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -788,10 +862,15 @@
         <f t="shared" si="0"/>
         <v>101011</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="8"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E5" s="13">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Opcode (hex)]])</f>
+        <v>43</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
@@ -805,10 +884,15 @@
         <f t="shared" si="0"/>
         <v>000100</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E6" s="13">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Opcode (hex)]])</f>
+        <v>4</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
@@ -822,10 +906,15 @@
         <f t="shared" si="0"/>
         <v>000101</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="13">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Opcode (hex)]])</f>
+        <v>5</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
@@ -839,10 +928,15 @@
         <f t="shared" si="0"/>
         <v>001000</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="13">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Opcode (hex)]])</f>
+        <v>8</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
@@ -856,10 +950,15 @@
         <f t="shared" si="0"/>
         <v>001111</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="8"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="13">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Opcode (hex)]])</f>
+        <v>15</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>23</v>
       </c>
@@ -873,10 +972,15 @@
         <f t="shared" si="0"/>
         <v>000010</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="8"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E10" s="13">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Opcode (hex)]])</f>
+        <v>2</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
@@ -890,10 +994,15 @@
         <f t="shared" si="0"/>
         <v>000011</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E11" s="13">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Opcode (hex)]])</f>
+        <v>3</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>27</v>
       </c>
@@ -907,15 +1016,23 @@
         <f t="shared" si="0"/>
         <v>000000</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="9" t="str">
-        <f t="shared" ref="F12:F27" si="1">HEX2BIN(E12,6)</f>
-        <v>000000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E12" s="13">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Opcode (hex)]])</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="6" t="str">
+        <f t="shared" ref="G12:G27" si="1">HEX2BIN(F12,6)</f>
+        <v>000000</v>
+      </c>
+      <c r="H12" s="15">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Func (hex)]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>30</v>
       </c>
@@ -929,15 +1046,23 @@
         <f t="shared" si="0"/>
         <v>000000</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="9" t="str">
+      <c r="E13" s="13">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Opcode (hex)]])</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="6" t="str">
         <f t="shared" si="1"/>
         <v>000000</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H13" s="15">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Func (hex)]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>31</v>
       </c>
@@ -951,15 +1076,23 @@
         <f t="shared" si="0"/>
         <v>000000</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="13">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Opcode (hex)]])</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="9" t="str">
+      <c r="G14" s="6" t="str">
         <f t="shared" si="1"/>
         <v>010000</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H14" s="15">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Func (hex)]])</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>33</v>
       </c>
@@ -973,15 +1106,23 @@
         <f t="shared" si="0"/>
         <v>000000</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="13">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Opcode (hex)]])</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="9" t="str">
+      <c r="G15" s="6" t="str">
         <f t="shared" si="1"/>
         <v>010010</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H15" s="15">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Func (hex)]])</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>35</v>
       </c>
@@ -995,15 +1136,23 @@
         <f t="shared" si="0"/>
         <v>000000</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="13">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Opcode (hex)]])</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="9" t="str">
+      <c r="G16" s="6" t="str">
         <f t="shared" si="1"/>
         <v>011000</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H16" s="15">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Func (hex)]])</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>37</v>
       </c>
@@ -1017,15 +1166,23 @@
         <f t="shared" si="0"/>
         <v>000000</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="13">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Opcode (hex)]])</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="9" t="str">
+      <c r="G17" s="6" t="str">
         <f t="shared" si="1"/>
         <v>011010</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H17" s="15">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Func (hex)]])</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>39</v>
       </c>
@@ -1039,15 +1196,23 @@
         <f t="shared" si="0"/>
         <v>000000</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="13">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Opcode (hex)]])</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="9" t="str">
+      <c r="G18" s="6" t="str">
         <f t="shared" si="1"/>
         <v>000010</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H18" s="15">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Func (hex)]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>40</v>
       </c>
@@ -1061,15 +1226,23 @@
         <f t="shared" si="0"/>
         <v>000000</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="13">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Opcode (hex)]])</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="9" t="str">
+      <c r="G19" s="6" t="str">
         <f t="shared" si="1"/>
         <v>100000</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H19" s="15">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Func (hex)]])</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>42</v>
       </c>
@@ -1083,15 +1256,23 @@
         <f t="shared" si="0"/>
         <v>000000</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="13">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Opcode (hex)]])</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F20" s="9" t="str">
+      <c r="G20" s="6" t="str">
         <f t="shared" si="1"/>
         <v>100010</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H20" s="15">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Func (hex)]])</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>44</v>
       </c>
@@ -1105,15 +1286,23 @@
         <f t="shared" si="0"/>
         <v>000000</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="13">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Opcode (hex)]])</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F21" s="9" t="str">
+      <c r="G21" s="6" t="str">
         <f t="shared" si="1"/>
         <v>100100</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H21" s="15">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Func (hex)]])</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>46</v>
       </c>
@@ -1127,15 +1316,23 @@
         <f t="shared" si="0"/>
         <v>000000</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="13">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Opcode (hex)]])</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F22" s="9" t="str">
+      <c r="G22" s="6" t="str">
         <f t="shared" si="1"/>
         <v>100101</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H22" s="15">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Func (hex)]])</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>48</v>
       </c>
@@ -1149,15 +1346,23 @@
         <f t="shared" si="0"/>
         <v>000000</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="13">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Opcode (hex)]])</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F23" s="9" t="str">
+      <c r="G23" s="6" t="str">
         <f t="shared" si="1"/>
         <v>100110</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H23" s="15">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Func (hex)]])</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>50</v>
       </c>
@@ -1171,15 +1376,23 @@
         <f t="shared" si="0"/>
         <v>000000</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="13">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Opcode (hex)]])</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F24" s="9" t="str">
+      <c r="G24" s="6" t="str">
         <f t="shared" si="1"/>
         <v>101010</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H24" s="15">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Func (hex)]])</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>52</v>
       </c>
@@ -1193,15 +1406,23 @@
         <f t="shared" si="0"/>
         <v>000000</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="13">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Opcode (hex)]])</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F25" s="9" t="str">
+      <c r="G25" s="6" t="str">
         <f t="shared" si="1"/>
         <v>001000</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H25" s="15">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Func (hex)]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>53</v>
       </c>
@@ -1215,40 +1436,57 @@
         <f t="shared" si="0"/>
         <v>000000</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E26" s="13">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Opcode (hex)]])</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F26" s="9" t="str">
+      <c r="G26" s="6" t="str">
         <f t="shared" si="1"/>
         <v>010010</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="s">
+      <c r="H26" s="15">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Func (hex)]])</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D27" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>000000</v>
-      </c>
-      <c r="E27" s="12" t="s">
+      <c r="C27" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>000000</v>
+      </c>
+      <c r="E27" s="14">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Opcode (hex)]])</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="13" t="str">
+      <c r="G27" s="11" t="str">
         <f t="shared" si="1"/>
         <v>000010</v>
       </c>
+      <c r="H27" s="16">
+        <f>HEX2DEC(__Anonymous_Sheet_DB__0[[#This Row],[Func (hex)]])</f>
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>